<commit_message>
Nueva hoja informe errores en plantillas
</commit_message>
<xml_diff>
--- a/plantillas/Anexo Informe Revision Accesibilidad - Aplicaciones moviles.xlsx
+++ b/plantillas/Anexo Informe Revision Accesibilidad - Aplicaciones moviles.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseR\Mi unidad\curso2021-2022\accesibilidad Castellon\Modelos para informes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\accesibilidad\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FB15AE-912C-4CD7-A17A-F06980206C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B346407-652A-452A-A069-0F4FAB6A2343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="45" r:id="rId1"/>
     <sheet name="Comentarios" sheetId="48" r:id="rId2"/>
     <sheet name="Declaración" sheetId="47" r:id="rId3"/>
+    <sheet name="Informe Errores" sheetId="49" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Comentarios!$A$1:$J$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Informe Errores'!$A$1:$F$138</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Procesos!$A$1:$C$14</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -130,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="194">
   <si>
     <t>5.2 Activación de características de accesibilidad</t>
   </si>
@@ -715,6 +717,15 @@
   </si>
   <si>
     <t>Núm. Requisito en Tabla A.2 de la norma</t>
+  </si>
+  <si>
+    <t>Localización del problema (página/s de la muestra)</t>
+  </si>
+  <si>
+    <t>Descripción del problema (opcional: capturas de pantalla)</t>
+  </si>
+  <si>
+    <t>Propuesta de solución</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4451,4 +4462,2323 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293081B4-7007-4BE0-9A3A-3BD73CDD4B6D}">
+  <dimension ref="A1:F163"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="96.6">
+      <c r="A1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="39.6">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" ht="52.8">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15">
+        <v>3</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" ht="26.4">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15">
+        <v>4</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" ht="39.6">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>5</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.4">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
+        <v>7</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="26.4">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <v>8</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" ht="26.4">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15">
+        <v>9</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="26.4">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15">
+        <v>10</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" ht="26.4">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15">
+        <v>11</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" ht="26.4">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15">
+        <v>12</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" ht="26.4">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15">
+        <v>13</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" ht="39.6">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" ht="52.8">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15">
+        <v>15</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" ht="26.4">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15">
+        <v>16</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" ht="26.4">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15">
+        <v>17</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="13">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15">
+        <v>18</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="13">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15">
+        <v>19</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="13">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15">
+        <v>20</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="13">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15">
+        <v>21</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" ht="39.6">
+      <c r="A23" s="13">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15">
+        <v>22</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" ht="26.4">
+      <c r="A24" s="13">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15">
+        <v>23</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" ht="26.4">
+      <c r="A25" s="13">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15">
+        <v>24</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="13">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15">
+        <v>25</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="1:6" ht="26.4">
+      <c r="A27" s="13">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15">
+        <v>26</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:6" ht="26.4">
+      <c r="A28" s="13">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15">
+        <v>27</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:6" ht="26.4">
+      <c r="A29" s="13">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15">
+        <v>28</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="1:6" ht="52.8">
+      <c r="A30" s="13">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15">
+        <v>29</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="1:6" ht="26.4">
+      <c r="A31" s="13">
+        <v>30</v>
+      </c>
+      <c r="B31" s="15">
+        <v>30</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="1:6" ht="26.4">
+      <c r="A32" s="13">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15">
+        <v>31</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="1:6" ht="26.4">
+      <c r="A33" s="13">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15">
+        <v>32</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+    </row>
+    <row r="34" spans="1:6" ht="26.4">
+      <c r="A34" s="13">
+        <v>33</v>
+      </c>
+      <c r="B34" s="15">
+        <v>33</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="13">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15">
+        <v>34</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+    </row>
+    <row r="36" spans="1:6" ht="26.4">
+      <c r="A36" s="13">
+        <v>35</v>
+      </c>
+      <c r="B36" s="15">
+        <v>35</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+    </row>
+    <row r="37" spans="1:6" ht="26.4">
+      <c r="A37" s="13">
+        <v>36</v>
+      </c>
+      <c r="B37" s="15">
+        <v>36</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+    </row>
+    <row r="38" spans="1:6" ht="26.4">
+      <c r="A38" s="13">
+        <v>37</v>
+      </c>
+      <c r="B38" s="15">
+        <v>37</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+    </row>
+    <row r="39" spans="1:6" ht="39.6">
+      <c r="A39" s="13">
+        <v>38</v>
+      </c>
+      <c r="B39" s="15">
+        <v>38</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+    </row>
+    <row r="40" spans="1:6" ht="26.4">
+      <c r="A40" s="13">
+        <v>39</v>
+      </c>
+      <c r="B40" s="15">
+        <v>39</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+    </row>
+    <row r="41" spans="1:6" ht="26.4">
+      <c r="A41" s="13">
+        <v>40</v>
+      </c>
+      <c r="B41" s="15">
+        <v>40</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+    </row>
+    <row r="42" spans="1:6" ht="26.4">
+      <c r="A42" s="13">
+        <v>41</v>
+      </c>
+      <c r="B42" s="15">
+        <v>41</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+    </row>
+    <row r="43" spans="1:6" ht="52.8">
+      <c r="A43" s="13">
+        <v>42</v>
+      </c>
+      <c r="B43" s="15">
+        <v>42</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+    </row>
+    <row r="44" spans="1:6" ht="39.6">
+      <c r="A44" s="13">
+        <v>43</v>
+      </c>
+      <c r="B44" s="15">
+        <v>43</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+    </row>
+    <row r="45" spans="1:6" ht="26.4">
+      <c r="A45" s="13">
+        <v>44</v>
+      </c>
+      <c r="B45" s="15">
+        <v>44</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="18"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+    </row>
+    <row r="46" spans="1:6" ht="26.4">
+      <c r="A46" s="13">
+        <v>45</v>
+      </c>
+      <c r="B46" s="15">
+        <v>45</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="18"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+    </row>
+    <row r="47" spans="1:6" ht="26.4">
+      <c r="A47" s="13">
+        <v>46</v>
+      </c>
+      <c r="B47" s="15">
+        <v>46</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="18"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="13">
+        <v>47</v>
+      </c>
+      <c r="B48" s="15">
+        <v>47</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+    </row>
+    <row r="49" spans="1:6" ht="39.6">
+      <c r="A49" s="13">
+        <v>48</v>
+      </c>
+      <c r="B49" s="15">
+        <v>48</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="18"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="13">
+        <v>49</v>
+      </c>
+      <c r="B50" s="15">
+        <v>49</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="18"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+    </row>
+    <row r="51" spans="1:6" ht="26.4">
+      <c r="A51" s="13">
+        <v>50</v>
+      </c>
+      <c r="B51" s="15">
+        <v>50</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" spans="1:6" ht="26.4">
+      <c r="A52" s="13">
+        <v>51</v>
+      </c>
+      <c r="B52" s="15">
+        <v>51</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="18"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+    </row>
+    <row r="53" spans="1:6" ht="26.4">
+      <c r="A53" s="13">
+        <v>52</v>
+      </c>
+      <c r="B53" s="15">
+        <v>52</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="18"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+    </row>
+    <row r="54" spans="1:6" ht="26.4">
+      <c r="A54" s="13">
+        <v>53</v>
+      </c>
+      <c r="B54" s="15">
+        <v>53</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="18"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+    </row>
+    <row r="55" spans="1:6" ht="26.4">
+      <c r="A55" s="13">
+        <v>54</v>
+      </c>
+      <c r="B55" s="15">
+        <v>54</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="18"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+    </row>
+    <row r="56" spans="1:6" ht="26.4">
+      <c r="A56" s="13">
+        <v>55</v>
+      </c>
+      <c r="B56" s="15">
+        <v>55</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="18"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+    </row>
+    <row r="57" spans="1:6" ht="26.4">
+      <c r="A57" s="13">
+        <v>56</v>
+      </c>
+      <c r="B57" s="15">
+        <v>56</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="18"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+    </row>
+    <row r="58" spans="1:6" ht="39.6">
+      <c r="A58" s="13">
+        <v>57</v>
+      </c>
+      <c r="B58" s="15">
+        <v>57</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="13">
+        <v>58</v>
+      </c>
+      <c r="B59" s="15">
+        <v>58</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="18"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+    </row>
+    <row r="60" spans="1:6" ht="26.4">
+      <c r="A60" s="13">
+        <v>59</v>
+      </c>
+      <c r="B60" s="15">
+        <v>59</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="18"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+    </row>
+    <row r="61" spans="1:6" ht="26.4">
+      <c r="A61" s="13">
+        <v>60</v>
+      </c>
+      <c r="B61" s="15">
+        <v>60</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="18"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+    </row>
+    <row r="62" spans="1:6" ht="26.4">
+      <c r="A62" s="13">
+        <v>61</v>
+      </c>
+      <c r="B62" s="15">
+        <v>61</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+    </row>
+    <row r="63" spans="1:6" ht="26.4">
+      <c r="A63" s="13">
+        <v>62</v>
+      </c>
+      <c r="B63" s="15">
+        <v>62</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" s="18"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="64" spans="1:6" ht="26.4">
+      <c r="A64" s="13">
+        <v>63</v>
+      </c>
+      <c r="B64" s="15">
+        <v>63</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64" s="18"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+    </row>
+    <row r="65" spans="1:6" ht="26.4">
+      <c r="A65" s="13">
+        <v>64</v>
+      </c>
+      <c r="B65" s="15">
+        <v>64</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" s="18"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="13">
+        <v>65</v>
+      </c>
+      <c r="B66" s="15">
+        <v>65</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D66" s="18"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+    </row>
+    <row r="67" spans="1:6" ht="26.4">
+      <c r="A67" s="13">
+        <v>66</v>
+      </c>
+      <c r="B67" s="15">
+        <v>66</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67" s="18"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+    </row>
+    <row r="68" spans="1:6" ht="26.4">
+      <c r="A68" s="13">
+        <v>67</v>
+      </c>
+      <c r="B68" s="15">
+        <v>67</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68" s="18"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="13">
+        <v>68</v>
+      </c>
+      <c r="B69" s="15">
+        <v>68</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="18"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+    </row>
+    <row r="70" spans="1:6" ht="26.4">
+      <c r="A70" s="13">
+        <v>69</v>
+      </c>
+      <c r="B70" s="15">
+        <v>69</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="18"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+    </row>
+    <row r="71" spans="1:6" ht="26.4">
+      <c r="A71" s="13">
+        <v>70</v>
+      </c>
+      <c r="B71" s="15">
+        <v>70</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+    </row>
+    <row r="72" spans="1:6" ht="26.4">
+      <c r="A72" s="13">
+        <v>71</v>
+      </c>
+      <c r="B72" s="15">
+        <v>71</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+    </row>
+    <row r="73" spans="1:6" ht="26.4">
+      <c r="A73" s="13">
+        <v>72</v>
+      </c>
+      <c r="B73" s="15">
+        <v>72</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="18"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+    </row>
+    <row r="74" spans="1:6" ht="26.4">
+      <c r="A74" s="13">
+        <v>73</v>
+      </c>
+      <c r="B74" s="15">
+        <v>73</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D74" s="18"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+    </row>
+    <row r="75" spans="1:6" ht="26.4">
+      <c r="A75" s="13">
+        <v>74</v>
+      </c>
+      <c r="B75" s="15">
+        <v>74</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="18"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+    </row>
+    <row r="76" spans="1:6" ht="26.4">
+      <c r="A76" s="13">
+        <v>75</v>
+      </c>
+      <c r="B76" s="15">
+        <v>75</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D76" s="18"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+    </row>
+    <row r="77" spans="1:6" ht="26.4">
+      <c r="A77" s="13">
+        <v>76</v>
+      </c>
+      <c r="B77" s="15">
+        <v>76</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="18"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+    </row>
+    <row r="78" spans="1:6" ht="26.4">
+      <c r="A78" s="13">
+        <v>77</v>
+      </c>
+      <c r="B78" s="15">
+        <v>77</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+    </row>
+    <row r="79" spans="1:6" ht="26.4">
+      <c r="A79" s="13">
+        <v>78</v>
+      </c>
+      <c r="B79" s="15">
+        <v>78</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+    </row>
+    <row r="80" spans="1:6" ht="26.4">
+      <c r="A80" s="13">
+        <v>79</v>
+      </c>
+      <c r="B80" s="15">
+        <v>79</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+    </row>
+    <row r="81" spans="1:6" ht="39.6">
+      <c r="A81" s="13">
+        <v>80</v>
+      </c>
+      <c r="B81" s="15">
+        <v>80</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D81" s="18"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="13">
+        <v>81</v>
+      </c>
+      <c r="B82" s="15">
+        <v>81</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+    </row>
+    <row r="83" spans="1:6" ht="26.4">
+      <c r="A83" s="13">
+        <v>82</v>
+      </c>
+      <c r="B83" s="15">
+        <v>82</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+    </row>
+    <row r="84" spans="1:6" ht="26.4">
+      <c r="A84" s="13">
+        <v>83</v>
+      </c>
+      <c r="B84" s="15">
+        <v>83</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D84" s="18"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+    </row>
+    <row r="85" spans="1:6" ht="39.6">
+      <c r="A85" s="13">
+        <v>84</v>
+      </c>
+      <c r="B85" s="15">
+        <v>84</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85" s="18"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+    </row>
+    <row r="86" spans="1:6" ht="39.6">
+      <c r="A86" s="13">
+        <v>85</v>
+      </c>
+      <c r="B86" s="15">
+        <v>85</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D86" s="18"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+    </row>
+    <row r="87" spans="1:6" ht="39.6">
+      <c r="A87" s="13">
+        <v>86</v>
+      </c>
+      <c r="B87" s="15">
+        <v>86</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+    </row>
+    <row r="88" spans="1:6" ht="39.6">
+      <c r="A88" s="13">
+        <v>87</v>
+      </c>
+      <c r="B88" s="15">
+        <v>87</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+    </row>
+    <row r="89" spans="1:6" ht="26.4">
+      <c r="A89" s="13">
+        <v>88</v>
+      </c>
+      <c r="B89" s="15">
+        <v>88</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+    </row>
+    <row r="90" spans="1:6" ht="66">
+      <c r="A90" s="13">
+        <v>89</v>
+      </c>
+      <c r="B90" s="15">
+        <v>89</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+    </row>
+    <row r="91" spans="1:6" ht="66">
+      <c r="A91" s="13">
+        <v>90</v>
+      </c>
+      <c r="B91" s="15">
+        <v>90</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+    </row>
+    <row r="92" spans="1:6" ht="39.6">
+      <c r="A92" s="13">
+        <v>91</v>
+      </c>
+      <c r="B92" s="15">
+        <v>91</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92" s="18"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+    </row>
+    <row r="93" spans="1:6" ht="39.6">
+      <c r="A93" s="13">
+        <v>92</v>
+      </c>
+      <c r="B93" s="15">
+        <v>92</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+    </row>
+    <row r="94" spans="1:6" ht="39.6">
+      <c r="A94" s="13">
+        <v>93</v>
+      </c>
+      <c r="B94" s="15">
+        <v>93</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+    </row>
+    <row r="95" spans="1:6" ht="26.4">
+      <c r="A95" s="13">
+        <v>94</v>
+      </c>
+      <c r="B95" s="15">
+        <v>94</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="13">
+        <v>95</v>
+      </c>
+      <c r="B96" s="15">
+        <v>95</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D96" s="18"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+    </row>
+    <row r="97" spans="1:6" ht="52.8">
+      <c r="A97" s="13">
+        <v>96</v>
+      </c>
+      <c r="B97" s="15">
+        <v>96</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D97" s="18"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+    </row>
+    <row r="98" spans="1:6" ht="52.8">
+      <c r="A98" s="13">
+        <v>97</v>
+      </c>
+      <c r="B98" s="15">
+        <v>97</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="13">
+        <v>98</v>
+      </c>
+      <c r="B99" s="15">
+        <v>98</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D99" s="18"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+    </row>
+    <row r="100" spans="1:6" ht="26.4">
+      <c r="A100" s="13">
+        <v>99</v>
+      </c>
+      <c r="B100" s="15">
+        <v>99</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D100" s="18"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+    </row>
+    <row r="101" spans="1:6" ht="26.4">
+      <c r="A101" s="13">
+        <v>100</v>
+      </c>
+      <c r="B101" s="15">
+        <v>100</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D101" s="18"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+    </row>
+    <row r="102" spans="1:6" ht="39.6">
+      <c r="A102" s="13">
+        <v>101</v>
+      </c>
+      <c r="B102" s="15">
+        <v>101</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D102" s="18"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+    </row>
+    <row r="103" spans="1:6" ht="39.6">
+      <c r="A103" s="13">
+        <v>102</v>
+      </c>
+      <c r="B103" s="15">
+        <v>102</v>
+      </c>
+      <c r="C103" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D103" s="18"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+    </row>
+    <row r="104" spans="1:6" ht="39.6">
+      <c r="A104" s="13">
+        <v>103</v>
+      </c>
+      <c r="B104" s="15">
+        <v>103</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D104" s="18"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+    </row>
+    <row r="105" spans="1:6" ht="39.6">
+      <c r="A105" s="13">
+        <v>104</v>
+      </c>
+      <c r="B105" s="15">
+        <v>104</v>
+      </c>
+      <c r="C105" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D105" s="18"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+    </row>
+    <row r="106" spans="1:6" ht="26.4">
+      <c r="A106" s="13">
+        <v>105</v>
+      </c>
+      <c r="B106" s="15">
+        <v>105</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D106" s="18"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+    </row>
+    <row r="107" spans="1:6" ht="26.4">
+      <c r="A107" s="13">
+        <v>106</v>
+      </c>
+      <c r="B107" s="15">
+        <v>106</v>
+      </c>
+      <c r="C107" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D107" s="18"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+    </row>
+    <row r="108" spans="1:6" ht="26.4">
+      <c r="A108" s="13">
+        <v>107</v>
+      </c>
+      <c r="B108" s="15">
+        <v>107</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D108" s="18"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+    </row>
+    <row r="109" spans="1:6" ht="39.6">
+      <c r="A109" s="13">
+        <v>108</v>
+      </c>
+      <c r="B109" s="15">
+        <v>108</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D109" s="18"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+    </row>
+    <row r="110" spans="1:6" ht="26.4">
+      <c r="A110" s="13">
+        <v>109</v>
+      </c>
+      <c r="B110" s="15">
+        <v>109</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D110" s="18"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+    </row>
+    <row r="111" spans="1:6" ht="26.4">
+      <c r="A111" s="13">
+        <v>110</v>
+      </c>
+      <c r="B111" s="15">
+        <v>110</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D111" s="18"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+    </row>
+    <row r="112" spans="1:6" ht="26.4">
+      <c r="A112" s="13">
+        <v>111</v>
+      </c>
+      <c r="B112" s="15">
+        <v>111</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D112" s="18"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+    </row>
+    <row r="113" spans="1:6" ht="39.6">
+      <c r="A113" s="13">
+        <v>112</v>
+      </c>
+      <c r="B113" s="15">
+        <v>112</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D113" s="18"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+    </row>
+    <row r="114" spans="1:6" ht="39.6">
+      <c r="A114" s="13">
+        <v>113</v>
+      </c>
+      <c r="B114" s="15">
+        <v>113</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D114" s="18"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+    </row>
+    <row r="115" spans="1:6" ht="26.4">
+      <c r="A115" s="13">
+        <v>114</v>
+      </c>
+      <c r="B115" s="15">
+        <v>114</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D115" s="18"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+    </row>
+    <row r="116" spans="1:6" ht="26.4">
+      <c r="A116" s="13">
+        <v>115</v>
+      </c>
+      <c r="B116" s="15">
+        <v>115</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D116" s="18"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+    </row>
+    <row r="117" spans="1:6" ht="26.4">
+      <c r="A117" s="13">
+        <v>116</v>
+      </c>
+      <c r="B117" s="15">
+        <v>116</v>
+      </c>
+      <c r="C117" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D117" s="18"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="13">
+        <v>117</v>
+      </c>
+      <c r="B118" s="15">
+        <v>117</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D118" s="18"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+    </row>
+    <row r="119" spans="1:6" ht="26.4">
+      <c r="A119" s="13">
+        <v>118</v>
+      </c>
+      <c r="B119" s="15">
+        <v>118</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D119" s="18"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+    </row>
+    <row r="120" spans="1:6" ht="26.4">
+      <c r="A120" s="13">
+        <v>119</v>
+      </c>
+      <c r="B120" s="15">
+        <v>119</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D120" s="18"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="13">
+        <v>120</v>
+      </c>
+      <c r="B121" s="15">
+        <v>120</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D121" s="18"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+    </row>
+    <row r="122" spans="1:6" ht="26.4">
+      <c r="A122" s="13">
+        <v>121</v>
+      </c>
+      <c r="B122" s="15">
+        <v>121</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D122" s="18"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+    </row>
+    <row r="123" spans="1:6" ht="26.4">
+      <c r="A123" s="13">
+        <v>122</v>
+      </c>
+      <c r="B123" s="15">
+        <v>122</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D123" s="18"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="19"/>
+    </row>
+    <row r="124" spans="1:6" ht="39.6">
+      <c r="A124" s="13">
+        <v>123</v>
+      </c>
+      <c r="B124" s="15">
+        <v>123</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D124" s="18"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="19"/>
+    </row>
+    <row r="125" spans="1:6" ht="26.4">
+      <c r="A125" s="13">
+        <v>124</v>
+      </c>
+      <c r="B125" s="15">
+        <v>124</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D125" s="18"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="19"/>
+    </row>
+    <row r="126" spans="1:6" ht="39.6">
+      <c r="A126" s="13">
+        <v>125</v>
+      </c>
+      <c r="B126" s="15">
+        <v>125</v>
+      </c>
+      <c r="C126" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D126" s="18"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="19"/>
+    </row>
+    <row r="127" spans="1:6" ht="39.6">
+      <c r="A127" s="13">
+        <v>126</v>
+      </c>
+      <c r="B127" s="15">
+        <v>126</v>
+      </c>
+      <c r="C127" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D127" s="18"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="19"/>
+    </row>
+    <row r="128" spans="1:6" ht="26.4">
+      <c r="A128" s="13">
+        <v>127</v>
+      </c>
+      <c r="B128" s="15">
+        <v>127</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D128" s="18"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="19"/>
+    </row>
+    <row r="129" spans="1:6" ht="26.4">
+      <c r="A129" s="13">
+        <v>128</v>
+      </c>
+      <c r="B129" s="15">
+        <v>128</v>
+      </c>
+      <c r="C129" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D129" s="18"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19"/>
+    </row>
+    <row r="130" spans="1:6" ht="39.6">
+      <c r="A130" s="13">
+        <v>129</v>
+      </c>
+      <c r="B130" s="15">
+        <v>129</v>
+      </c>
+      <c r="C130" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D130" s="18"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="19"/>
+    </row>
+    <row r="131" spans="1:6" ht="39.6">
+      <c r="A131" s="13">
+        <v>130</v>
+      </c>
+      <c r="B131" s="15">
+        <v>130</v>
+      </c>
+      <c r="C131" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D131" s="18"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="19"/>
+    </row>
+    <row r="132" spans="1:6" ht="26.4">
+      <c r="A132" s="13">
+        <v>131</v>
+      </c>
+      <c r="B132" s="15">
+        <v>131</v>
+      </c>
+      <c r="C132" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D132" s="18"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="19"/>
+    </row>
+    <row r="133" spans="1:6" ht="26.4">
+      <c r="A133" s="13">
+        <v>132</v>
+      </c>
+      <c r="B133" s="15">
+        <v>132</v>
+      </c>
+      <c r="C133" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D133" s="18"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="19"/>
+    </row>
+    <row r="134" spans="1:6" ht="39.6">
+      <c r="A134" s="13">
+        <v>133</v>
+      </c>
+      <c r="B134" s="15">
+        <v>133</v>
+      </c>
+      <c r="C134" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D134" s="18"/>
+      <c r="E134" s="19"/>
+      <c r="F134" s="19"/>
+    </row>
+    <row r="135" spans="1:6" ht="39.6">
+      <c r="A135" s="13">
+        <v>134</v>
+      </c>
+      <c r="B135" s="15">
+        <v>134</v>
+      </c>
+      <c r="C135" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D135" s="18"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="19"/>
+    </row>
+    <row r="136" spans="1:6" ht="39.6">
+      <c r="A136" s="13">
+        <v>135</v>
+      </c>
+      <c r="B136" s="15">
+        <v>135</v>
+      </c>
+      <c r="C136" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D136" s="18"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="19"/>
+    </row>
+    <row r="137" spans="1:6" ht="39.6">
+      <c r="A137" s="13">
+        <v>136</v>
+      </c>
+      <c r="B137" s="15">
+        <v>136</v>
+      </c>
+      <c r="C137" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D137" s="18"/>
+      <c r="E137" s="19"/>
+      <c r="F137" s="19"/>
+    </row>
+    <row r="138" spans="1:6" ht="39.6">
+      <c r="A138" s="13">
+        <v>137</v>
+      </c>
+      <c r="B138" s="15">
+        <v>137</v>
+      </c>
+      <c r="C138" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D138" s="18"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+    </row>
+    <row r="139" spans="1:6" ht="26.4">
+      <c r="A139" s="13">
+        <v>138</v>
+      </c>
+      <c r="B139" s="15">
+        <v>138</v>
+      </c>
+      <c r="C139" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D139" s="19"/>
+      <c r="E139" s="19"/>
+      <c r="F139" s="19"/>
+    </row>
+    <row r="140" spans="1:6" ht="26.4">
+      <c r="A140" s="13">
+        <v>139</v>
+      </c>
+      <c r="B140" s="15">
+        <v>139</v>
+      </c>
+      <c r="C140" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D140" s="19"/>
+      <c r="E140" s="19"/>
+      <c r="F140" s="19"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="13">
+        <v>140</v>
+      </c>
+      <c r="B141" s="15">
+        <v>140</v>
+      </c>
+      <c r="C141" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D141" s="19"/>
+      <c r="E141" s="19"/>
+      <c r="F141" s="19"/>
+    </row>
+    <row r="142" spans="1:6" ht="26.4">
+      <c r="A142" s="13">
+        <v>141</v>
+      </c>
+      <c r="B142" s="15">
+        <v>141</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D142" s="19"/>
+      <c r="E142" s="19"/>
+      <c r="F142" s="19"/>
+    </row>
+    <row r="143" spans="1:6" ht="26.4">
+      <c r="A143" s="13">
+        <v>142</v>
+      </c>
+      <c r="B143" s="15">
+        <v>142</v>
+      </c>
+      <c r="C143" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D143" s="19"/>
+      <c r="E143" s="19"/>
+      <c r="F143" s="19"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="13">
+        <v>143</v>
+      </c>
+      <c r="B144" s="15">
+        <v>143</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D144" s="19"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="19"/>
+    </row>
+    <row r="145" spans="1:6" ht="26.4">
+      <c r="A145" s="13">
+        <v>144</v>
+      </c>
+      <c r="B145" s="15">
+        <v>144</v>
+      </c>
+      <c r="C145" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D145" s="19"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="19"/>
+    </row>
+    <row r="146" spans="1:6" ht="26.4">
+      <c r="A146" s="13">
+        <v>145</v>
+      </c>
+      <c r="B146" s="15">
+        <v>145</v>
+      </c>
+      <c r="C146" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D146" s="19"/>
+      <c r="E146" s="19"/>
+      <c r="F146" s="19"/>
+    </row>
+    <row r="147" spans="1:6" ht="39.6">
+      <c r="A147" s="13">
+        <v>146</v>
+      </c>
+      <c r="B147" s="15">
+        <v>146</v>
+      </c>
+      <c r="C147" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D147" s="19"/>
+      <c r="E147" s="19"/>
+      <c r="F147" s="19"/>
+    </row>
+    <row r="148" spans="1:6" ht="39.6">
+      <c r="A148" s="13">
+        <v>147</v>
+      </c>
+      <c r="B148" s="15">
+        <v>147</v>
+      </c>
+      <c r="C148" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D148" s="19"/>
+      <c r="E148" s="19"/>
+      <c r="F148" s="19"/>
+    </row>
+    <row r="149" spans="1:6" ht="26.4">
+      <c r="A149" s="13">
+        <v>148</v>
+      </c>
+      <c r="B149" s="15">
+        <v>148</v>
+      </c>
+      <c r="C149" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D149" s="19"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="19"/>
+    </row>
+    <row r="150" spans="1:6" ht="39.6">
+      <c r="A150" s="13">
+        <v>149</v>
+      </c>
+      <c r="B150" s="15">
+        <v>149</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D150" s="19"/>
+      <c r="E150" s="19"/>
+      <c r="F150" s="19"/>
+    </row>
+    <row r="151" spans="1:6" ht="26.4">
+      <c r="A151" s="13">
+        <v>150</v>
+      </c>
+      <c r="B151" s="15">
+        <v>150</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D151" s="19"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="19"/>
+    </row>
+    <row r="152" spans="1:6" ht="39.6">
+      <c r="A152" s="13">
+        <v>151</v>
+      </c>
+      <c r="B152" s="15">
+        <v>151</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D152" s="19"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="19"/>
+    </row>
+    <row r="153" spans="1:6" ht="26.4">
+      <c r="A153" s="13">
+        <v>152</v>
+      </c>
+      <c r="B153" s="15">
+        <v>152</v>
+      </c>
+      <c r="C153" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D153" s="19"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="19"/>
+    </row>
+    <row r="154" spans="1:6" ht="26.4">
+      <c r="A154" s="11">
+        <v>153</v>
+      </c>
+      <c r="B154" s="16">
+        <v>153</v>
+      </c>
+      <c r="C154" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="19"/>
+    </row>
+    <row r="155" spans="1:6" ht="26.4">
+      <c r="A155" s="11">
+        <v>154</v>
+      </c>
+      <c r="B155" s="16">
+        <v>154</v>
+      </c>
+      <c r="C155" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D155" s="19"/>
+      <c r="E155" s="19"/>
+      <c r="F155" s="19"/>
+    </row>
+    <row r="156" spans="1:6" ht="52.8">
+      <c r="A156" s="11">
+        <v>155</v>
+      </c>
+      <c r="B156" s="16">
+        <v>155</v>
+      </c>
+      <c r="C156" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D156" s="19"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="19"/>
+    </row>
+    <row r="157" spans="1:6" ht="26.4">
+      <c r="A157" s="11">
+        <v>156</v>
+      </c>
+      <c r="B157" s="16">
+        <v>156</v>
+      </c>
+      <c r="C157" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="19"/>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="11">
+        <v>157</v>
+      </c>
+      <c r="B158" s="16">
+        <v>157</v>
+      </c>
+      <c r="C158" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D158" s="19"/>
+      <c r="E158" s="19"/>
+      <c r="F158" s="19"/>
+    </row>
+    <row r="159" spans="1:6" ht="39.6">
+      <c r="A159" s="11">
+        <v>158</v>
+      </c>
+      <c r="B159" s="16">
+        <v>158</v>
+      </c>
+      <c r="C159" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D159" s="19"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="19"/>
+    </row>
+    <row r="160" spans="1:6" ht="26.4">
+      <c r="A160" s="11">
+        <v>159</v>
+      </c>
+      <c r="B160" s="16">
+        <v>159</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D160" s="19"/>
+      <c r="E160" s="19"/>
+      <c r="F160" s="19"/>
+    </row>
+    <row r="161" spans="1:6" ht="52.8">
+      <c r="A161" s="11">
+        <v>160</v>
+      </c>
+      <c r="B161" s="16">
+        <v>160</v>
+      </c>
+      <c r="C161" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D161" s="19"/>
+      <c r="E161" s="19"/>
+      <c r="F161" s="19"/>
+    </row>
+    <row r="162" spans="1:6" ht="26.4">
+      <c r="A162" s="11">
+        <v>161</v>
+      </c>
+      <c r="B162" s="16">
+        <v>161</v>
+      </c>
+      <c r="C162" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D162" s="19"/>
+      <c r="E162" s="19"/>
+      <c r="F162" s="19"/>
+    </row>
+    <row r="163" spans="1:6" ht="26.4">
+      <c r="A163" s="11">
+        <v>162</v>
+      </c>
+      <c r="B163" s="16">
+        <v>162</v>
+      </c>
+      <c r="C163" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" s="19"/>
+      <c r="E163" s="19"/>
+      <c r="F163" s="19"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F138" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E138" xr:uid="{7AC8011D-2D2A-4B15-B5C0-6D4DEC63C6DE}">
+      <formula1>",N/T,N/D,N/A,Falla,Pasa"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>